<commit_message>
Fixed typo in measurement template sample
</commit_message>
<xml_diff>
--- a/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/SampleMeasurementTemplate.xlsx
+++ b/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/SampleMeasurementTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/AIMSS/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964D740B-480D-4546-BCAA-EB7B84292709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96964F6-3305-F148-948F-6BBAEE8AC180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="6020" windowWidth="34320" windowHeight="18080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="780" windowWidth="34320" windowHeight="18080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t>DL_MESO</t>
   </si>
   <si>
-    <t>Numbe extra packages?</t>
-  </si>
-  <si>
     <t>Descriptive error messages?</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   </si>
   <si>
     <t>Overall impression (1..10)?</t>
+  </si>
+  <si>
+    <t>Number extra packages?</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:I26"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1102,7 +1102,7 @@
     <col min="10" max="10" width="12" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>34</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>37</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>37</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>37</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B19" s="21">
         <v>4</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>37</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>40</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B23" s="21">
         <v>9</v>
@@ -2083,7 +2083,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:9" ht="112" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" ht="98" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="42" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:12" ht="56" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>94</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Changes for the resubmitted version of the SOP of LBM
</commit_message>
<xml_diff>
--- a/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/SampleMeasurementTemplate.xlsx
+++ b/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/SampleMeasurementTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/AIMSS/StateOfPractice/Papers/LatticeBoltz_SOP-arXiv/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96964F6-3305-F148-948F-6BBAEE8AC180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EDB42-B054-694D-9951-08F96E6B0BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="780" windowWidth="34320" windowHeight="18080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="3900" windowWidth="34320" windowHeight="18080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t>DL_MESO</t>
   </si>
   <si>
-    <t>Descriptive error messages?</t>
-  </si>
-  <si>
     <t>Linear instructions?</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   </si>
   <si>
     <t>Number extra packages?</t>
+  </si>
+  <si>
+    <t>If install fails were there descriptive error messages?</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1344,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>34</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>37</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>37</v>
@@ -1508,9 +1508,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="8" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>37</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" s="21">
         <v>4</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>37</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>40</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B23" s="21">
         <v>9</v>

</xml_diff>